<commit_message>
Implementing pipelines for interacting with alert classification files
</commit_message>
<xml_diff>
--- a/epitweetr/inst/extdata/alert-training.xlsx
+++ b/epitweetr/inst/extdata/alert-training.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Alerts" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -71,6 +71,12 @@
     <t xml:space="preserve">FN</t>
   </si>
   <si>
+    <t xml:space="preserve">Precision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensitivity</t>
+  </si>
+  <si>
     <t xml:space="preserve">F1Score</t>
   </si>
   <si>
@@ -92,7 +98,7 @@
     <t xml:space="preserve">https://spark.apache.org/docs/3.0.1/api/scala/org/apache/spark/ml/classification/LinearSVC.html</t>
   </si>
   <si>
-    <t xml:space="preserve">{“regParam”:1, “tol”:0.1}</t>
+    <t xml:space="preserve">{"regParam":1, "tol":0.1}</t>
   </si>
   <si>
     <t xml:space="preserve">GBTClassifier</t>
@@ -123,6 +129,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -144,12 +151,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -307,11 +316,11 @@
   </sheetPr>
   <dimension ref="B2:I22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.78"/>
@@ -559,18 +568,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:M6"/>
+  <dimension ref="B3:O6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="26.13"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -610,13 +619,19 @@
       <c r="M3" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="N3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>2</v>
@@ -636,15 +651,22 @@
       <c r="I4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="3" t="b">
+      <c r="J4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>22</v>
+      <c r="N4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -652,7 +674,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>2</v>
@@ -672,15 +694,22 @@
       <c r="I5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="3" t="b">
+      <c r="J5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>25</v>
+      <c r="N5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -688,7 +717,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>2</v>
@@ -708,26 +737,33 @@
       <c r="I6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="3" t="b">
+      <c r="J6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="L6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>22</v>
+      <c r="N6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L4" r:id="rId1" display="https://spark.apache.org/docs/3.0.1/api/scala/org/apache/spark/ml/classification/LinearSVC.html"/>
-    <hyperlink ref="L5" r:id="rId2" display="https://spark.apache.org/docs/3.0.1/api/scala/org/apache/spark/ml/classification/GBTClassifier.html"/>
-    <hyperlink ref="L6" r:id="rId3" display="https://spark.apache.org/docs/3.0.1/api/scala/org/apache/spark/ml/classification/LogisticRegression.html"/>
+    <hyperlink ref="N4" r:id="rId1" display="https://spark.apache.org/docs/3.0.1/api/scala/org/apache/spark/ml/classification/LinearSVC.html"/>
+    <hyperlink ref="N5" r:id="rId2" display="https://spark.apache.org/docs/3.0.1/api/scala/org/apache/spark/ml/classification/GBTClassifier.html"/>
+    <hyperlink ref="N6" r:id="rId3" display="https://spark.apache.org/docs/3.0.1/api/scala/org/apache/spark/ml/classification/LogisticRegression.html"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
1. Finishing implementing ML for alerts, including subscriptors, retrain and search 2. Changing geotraining OK/KO to yes/no
</commit_message>
<xml_diff>
--- a/epitweetr/inst/extdata/alert-training.xlsx
+++ b/epitweetr/inst/extdata/alert-training.xlsx
@@ -11,20 +11,17 @@
     <sheet name="Alerts" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Runs" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName function="false" hidden="false" name="org.apache.spark.ml.param.DoubleParam" vbProcedure="false">#REF!</definedName>
-  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -56,30 +53,27 @@
     <t xml:space="preserve">Models</t>
   </si>
   <si>
+    <t xml:space="preserve">Alerts</t>
+  </si>
+  <si>
     <t xml:space="preserve">Runs</t>
   </si>
   <si>
-    <t xml:space="preserve">TP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Precision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sensitivity</t>
-  </si>
-  <si>
     <t xml:space="preserve">F1Score</t>
   </si>
   <si>
+    <t xml:space="preserve">Accuracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precision by Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensitivity by Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FScore by Class</t>
+  </si>
+  <si>
     <t xml:space="preserve">Last run</t>
   </si>
   <si>
@@ -92,13 +86,13 @@
     <t xml:space="preserve">Custom Parameters</t>
   </si>
   <si>
-    <t xml:space="preserve">Linear SVC</t>
+    <t xml:space="preserve">LinearSVC</t>
   </si>
   <si>
     <t xml:space="preserve">https://spark.apache.org/docs/3.0.1/api/scala/org/apache/spark/ml/classification/LinearSVC.html</t>
   </si>
   <si>
-    <t xml:space="preserve">{"regParam":1, "tol":0.1}</t>
+    <t xml:space="preserve">{"regParam":"1","tol":"0.1"}</t>
   </si>
   <si>
     <t xml:space="preserve">GBTClassifier</t>
@@ -120,14 +114,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="6">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -149,19 +143,20 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,8 +165,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <fgColor rgb="FFFF860D"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFDE59"/>
+        <bgColor rgb="FFFFCC00"/>
       </patternFill>
     </fill>
   </fills>
@@ -184,10 +185,10 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -221,16 +222,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -262,7 +263,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -287,12 +288,12 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFDE59"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF860D"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -303,10 +304,47 @@
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF222222"/>
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="A1:H51" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:H51"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Date"/>
+    <tableColumn id="2" name="Topic"/>
+    <tableColumn id="3" name="Region"/>
+    <tableColumn id="4" name="Top words"/>
+    <tableColumn id="5" name="Tweets"/>
+    <tableColumn id="6" name="Top Tweets"/>
+    <tableColumn id="7" name="Given Category"/>
+    <tableColumn id="8" name="Epitweetr Category"/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table4" displayName="Table4" ref="A1:M4" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:M4"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="Ranking"/>
+    <tableColumn id="2" name="Models"/>
+    <tableColumn id="3" name="Alerts"/>
+    <tableColumn id="4" name="Runs"/>
+    <tableColumn id="5" name="F1Score"/>
+    <tableColumn id="6" name="Accuracy"/>
+    <tableColumn id="7" name="Precision by Class"/>
+    <tableColumn id="8" name="Sensitivity by Class"/>
+    <tableColumn id="9" name="FScore by Class"/>
+    <tableColumn id="10" name="Last run"/>
+    <tableColumn id="11" name="Active"/>
+    <tableColumn id="12" name="Documentation"/>
+    <tableColumn id="13" name="Custom Parameters"/>
+  </tableColumns>
+</table>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -314,45 +352,49 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:I22"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="50.71"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="1" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -360,9 +402,9 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -370,9 +412,9 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -380,9 +422,9 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -390,9 +432,9 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -400,9 +442,9 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -410,9 +452,9 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -420,9 +462,9 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -430,9 +472,9 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -440,9 +482,9 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -450,9 +492,9 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -460,9 +502,9 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -470,9 +512,9 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -480,9 +522,9 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -490,9 +532,9 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -500,9 +542,9 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -510,9 +552,9 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -520,9 +562,9 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -530,9 +572,9 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -540,9 +582,9 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -550,16 +592,318 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
+  <tableParts>
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -568,205 +912,181 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:O6"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="26.13"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+    <row r="1" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2" t="n">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="E4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="3" t="n">
+      <c r="E2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="L2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="2" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="2" t="n">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="3" t="n">
+      <c r="E3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="L3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="2" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="2" t="n">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="E6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="3" t="n">
+      <c r="E4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="N6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>24</v>
+      <c r="L4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="N4" r:id="rId1" display="https://spark.apache.org/docs/3.0.1/api/scala/org/apache/spark/ml/classification/LinearSVC.html"/>
-    <hyperlink ref="N5" r:id="rId2" display="https://spark.apache.org/docs/3.0.1/api/scala/org/apache/spark/ml/classification/GBTClassifier.html"/>
-    <hyperlink ref="N6" r:id="rId3" display="https://spark.apache.org/docs/3.0.1/api/scala/org/apache/spark/ml/classification/LogisticRegression.html"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
+  <tableParts>
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>